<commit_message>
update task spreadsheet and meeting minutes
</commit_message>
<xml_diff>
--- a/Documentation/Project1TasksSpreadsheet.xlsx
+++ b/Documentation/Project1TasksSpreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="33960" windowHeight="22440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,106 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="78">
+  <si>
+    <t>Modify control loop for dynamic speed</t>
+  </si>
+  <si>
+    <t>Test dynamic speeds</t>
+  </si>
+  <si>
+    <t>Modify control loop to allow turning while moving</t>
+  </si>
+  <si>
+    <t>Test complete movement</t>
+  </si>
+  <si>
+    <t>Determine high level emergency stop implementation</t>
+  </si>
+  <si>
+    <t>Jerrell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Root Android Devices</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write code to send/receive stop command</t>
+  </si>
+  <si>
+    <t>Test stop code</t>
+  </si>
+  <si>
+    <t>%Complete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date Complete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Today:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Who</t>
+  </si>
+  <si>
+    <t>What</t>
+  </si>
+  <si>
+    <t>When</t>
+  </si>
+  <si>
+    <t>Sei Jung</t>
+  </si>
+  <si>
+    <t>Place phone case on phone</t>
+  </si>
+  <si>
+    <t>Learn to set up/compile code for Vex</t>
+  </si>
+  <si>
+    <t>Object Avoidance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android end of Vex-android communication</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vex end of Vex-android communication</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Controller</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Report</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grade Movement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jerrell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sei Jung/Jacob</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Jerrell</t>
   </si>
@@ -173,69 +272,6 @@
   </si>
   <si>
     <t>Calibrate speed based on joystick position</t>
-  </si>
-  <si>
-    <t>Modify control loop for dynamic speed</t>
-  </si>
-  <si>
-    <t>Test dynamic speeds</t>
-  </si>
-  <si>
-    <t>Modify control loop to allow turning while moving</t>
-  </si>
-  <si>
-    <t>Test complete movement</t>
-  </si>
-  <si>
-    <t>Determine high level emergency stop implementation</t>
-  </si>
-  <si>
-    <t>Jerrell</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Root Android Devices</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Write code to send/receive stop command</t>
-  </si>
-  <si>
-    <t>Test stop code</t>
-  </si>
-  <si>
-    <t>%Complete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Date Complete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Notes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Today:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Who</t>
-  </si>
-  <si>
-    <t>What</t>
-  </si>
-  <si>
-    <t>When</t>
-  </si>
-  <si>
-    <t>Sei Jung</t>
-  </si>
-  <si>
-    <t>Place phone case on phone</t>
-  </si>
-  <si>
-    <t>Learn to set up/compile code for Vex</t>
   </si>
 </sst>
 </file>
@@ -752,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -768,37 +804,37 @@
   <sheetData>
     <row r="1" spans="1:8" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="H1" s="7">
         <f ca="1">TODAY()</f>
-        <v>40067</v>
+        <v>40068</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14" thickBot="1">
       <c r="A2" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="C2" s="5">
         <v>40059</v>
@@ -817,10 +853,10 @@
     </row>
     <row r="3" spans="1:8" ht="14" thickBot="1">
       <c r="A3" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5">
         <v>40059</v>
@@ -839,10 +875,10 @@
     </row>
     <row r="4" spans="1:8" ht="14" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C4" s="5">
         <v>40059</v>
@@ -861,30 +897,32 @@
     </row>
     <row r="5" spans="1:8" ht="14" thickBot="1">
       <c r="A5" s="3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="C5" s="5">
         <v>40059</v>
       </c>
       <c r="D5" s="13">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="9">
+        <v>40061</v>
+      </c>
       <c r="F5" s="6"/>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="14" thickBot="1">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C6" s="5">
         <v>40059</v>
@@ -903,10 +941,10 @@
     </row>
     <row r="7" spans="1:8" ht="14" thickBot="1">
       <c r="A7" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C7" s="5">
         <v>40060</v>
@@ -925,10 +963,10 @@
     </row>
     <row r="8" spans="1:8" ht="14" thickBot="1">
       <c r="A8" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C8" s="5">
         <v>40060</v>
@@ -947,10 +985,10 @@
     </row>
     <row r="9" spans="1:8" ht="14" thickBot="1">
       <c r="A9" s="3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C9" s="5">
         <v>40061</v>
@@ -969,10 +1007,10 @@
     </row>
     <row r="10" spans="1:8" ht="14" thickBot="1">
       <c r="A10" s="3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C10" s="5">
         <v>40061</v>
@@ -980,7 +1018,9 @@
       <c r="D10" s="13">
         <v>1</v>
       </c>
-      <c r="E10" s="9"/>
+      <c r="E10" s="9">
+        <v>40061</v>
+      </c>
       <c r="F10" s="6"/>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
@@ -989,30 +1029,32 @@
     </row>
     <row r="11" spans="1:8" ht="14" thickBot="1">
       <c r="A11" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="C11" s="5">
         <v>40061</v>
       </c>
       <c r="D11" s="13">
-        <v>0</v>
-      </c>
-      <c r="E11" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="9">
+        <v>40061</v>
+      </c>
       <c r="F11" s="6"/>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="14" thickBot="1">
       <c r="A12" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C12" s="5">
         <v>40061</v>
@@ -1020,7 +1062,9 @@
       <c r="D12" s="13">
         <v>1</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="9">
+        <v>40061</v>
+      </c>
       <c r="F12" s="6"/>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
@@ -1029,10 +1073,10 @@
     </row>
     <row r="13" spans="1:8" ht="14" thickBot="1">
       <c r="A13" s="3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C13" s="5">
         <v>40061</v>
@@ -1040,7 +1084,9 @@
       <c r="D13" s="13">
         <v>1</v>
       </c>
-      <c r="E13" s="9"/>
+      <c r="E13" s="9">
+        <v>40061</v>
+      </c>
       <c r="F13" s="6"/>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
@@ -1049,10 +1095,10 @@
     </row>
     <row r="14" spans="1:8" ht="14" thickBot="1">
       <c r="A14" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="C14" s="5">
         <v>40061</v>
@@ -1071,10 +1117,10 @@
     </row>
     <row r="15" spans="1:8" ht="14" thickBot="1">
       <c r="A15" s="3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="C15" s="5">
         <v>40061</v>
@@ -1093,33 +1139,35 @@
     </row>
     <row r="16" spans="1:8" ht="14" thickBot="1">
       <c r="A16" s="3" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="C16" s="5">
         <v>40063</v>
       </c>
       <c r="D16" s="13">
-        <v>0</v>
-      </c>
-      <c r="E16" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="9">
+        <v>40062</v>
+      </c>
       <c r="F16" s="6"/>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="14" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14" thickBot="1">
       <c r="A17" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="D17" s="13">
         <v>0</v>
@@ -1131,12 +1179,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14" thickBot="1">
+    <row r="18" spans="1:9" ht="14" thickBot="1">
       <c r="A18" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C18" s="5">
         <v>40063</v>
@@ -1153,12 +1201,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14" thickBot="1">
+    <row r="19" spans="1:9" ht="14" thickBot="1">
       <c r="A19" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="C19" s="5">
         <v>40061</v>
@@ -1175,12 +1223,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14" thickBot="1">
+    <row r="20" spans="1:9" ht="14" thickBot="1">
       <c r="A20" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="C20" s="5">
         <v>40063</v>
@@ -1197,12 +1245,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14" thickBot="1">
+    <row r="21" spans="1:9" ht="14" thickBot="1">
       <c r="A21" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="C21" s="5">
         <v>40063</v>
@@ -1219,12 +1267,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14" thickBot="1">
+    <row r="22" spans="1:9" ht="14" thickBot="1">
       <c r="A22" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C22" s="5">
         <v>40063</v>
@@ -1241,12 +1289,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="14" thickBot="1">
+    <row r="23" spans="1:9" ht="14" thickBot="1">
       <c r="A23" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C23" s="5">
         <v>40063</v>
@@ -1263,12 +1311,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14" thickBot="1">
+    <row r="24" spans="1:9" ht="14" thickBot="1">
       <c r="A24" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C24" s="5">
         <v>40063</v>
@@ -1280,19 +1328,19 @@
         <v>40062</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14" thickBot="1">
+    <row r="25" spans="1:9" ht="14" thickBot="1">
       <c r="A25" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C25" s="5">
         <v>40063</v>
@@ -1309,12 +1357,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="14" thickBot="1">
+    <row r="26" spans="1:9" ht="14" thickBot="1">
       <c r="A26" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="C26" s="5">
         <v>40066</v>
@@ -1326,19 +1374,19 @@
         <v>40062</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="14" thickBot="1">
+    <row r="27" spans="1:9" ht="14" thickBot="1">
       <c r="A27" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="C27" s="5">
         <v>40066</v>
@@ -1352,13 +1400,19 @@
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="14" thickBot="1">
+      <c r="H27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="14" thickBot="1">
       <c r="A28" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="C28" s="5">
         <v>40069</v>
@@ -1372,13 +1426,19 @@
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="14" thickBot="1">
+      <c r="H28" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="14" thickBot="1">
       <c r="A29" s="3" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="C29" s="5">
         <v>40070</v>
@@ -1392,13 +1452,19 @@
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="14" thickBot="1">
+      <c r="H29" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="14" thickBot="1">
       <c r="A30" s="3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="C30" s="5">
         <v>40061</v>
@@ -1410,69 +1476,90 @@
         <v>40062</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="14" thickBot="1">
+      <c r="I30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="14" thickBot="1">
       <c r="A31" s="3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="C31" s="5">
         <v>40066</v>
       </c>
       <c r="D31" s="13">
-        <v>0</v>
-      </c>
-      <c r="E31" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="E31" s="9">
+        <v>40066</v>
+      </c>
       <c r="F31" s="6"/>
       <c r="G31">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="14" thickBot="1">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>26</v>
+      </c>
+      <c r="I31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="14" thickBot="1">
       <c r="A32" s="3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="C32" s="5">
         <v>40069</v>
       </c>
       <c r="D32" s="13">
-        <v>0.75</v>
-      </c>
-      <c r="E32" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="E32" s="9">
+        <v>40066</v>
+      </c>
       <c r="F32" s="6" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="14" thickBot="1">
       <c r="A33" s="3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C33" s="5">
         <v>40070</v>
       </c>
       <c r="D33" s="13">
-        <v>0</v>
-      </c>
-      <c r="E33" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="E33" s="9">
+        <v>40066</v>
+      </c>
       <c r="F33" s="6"/>
       <c r="G33">
         <f t="shared" ca="1" si="0"/>
@@ -1481,10 +1568,10 @@
     </row>
     <row r="34" spans="1:7" ht="14" thickBot="1">
       <c r="A34" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="C34" s="5">
         <v>40061</v>
@@ -1496,7 +1583,7 @@
         <v>40067</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="0"/>
@@ -1505,10 +1592,10 @@
     </row>
     <row r="35" spans="1:7" ht="14" thickBot="1">
       <c r="A35" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="C35" s="5">
         <v>40066</v>
@@ -1518,7 +1605,7 @@
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="6" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="0"/>
@@ -1527,10 +1614,10 @@
     </row>
     <row r="36" spans="1:7" ht="14" thickBot="1">
       <c r="A36" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="C36" s="5">
         <v>40069</v>
@@ -1547,10 +1634,10 @@
     </row>
     <row r="37" spans="1:7" ht="14" thickBot="1">
       <c r="A37" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C37" s="5">
         <v>40070</v>
@@ -1567,10 +1654,10 @@
     </row>
     <row r="38" spans="1:7" ht="14" thickBot="1">
       <c r="A38" s="3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C38" s="5">
         <v>40073</v>
@@ -1587,10 +1674,10 @@
     </row>
     <row r="39" spans="1:7" ht="14" thickBot="1">
       <c r="A39" s="3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="C39" s="5">
         <v>40074</v>
@@ -1607,10 +1694,10 @@
     </row>
     <row r="40" spans="1:7" ht="14" thickBot="1">
       <c r="A40" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="C40" s="5">
         <v>40076</v>
@@ -1627,10 +1714,10 @@
     </row>
     <row r="41" spans="1:7" ht="14" thickBot="1">
       <c r="A41" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="C41" s="5">
         <v>40076</v>
@@ -1647,10 +1734,10 @@
     </row>
     <row r="42" spans="1:7" ht="14" thickBot="1">
       <c r="A42" s="3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="C42" s="5">
         <v>40063</v>
@@ -1667,10 +1754,10 @@
     </row>
     <row r="43" spans="1:7" ht="14" thickBot="1">
       <c r="A43" s="3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="C43" s="5">
         <v>40069</v>
@@ -1687,10 +1774,10 @@
     </row>
     <row r="44" spans="1:7" ht="14" thickBot="1">
       <c r="A44" s="3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="C44" s="5">
         <v>40069</v>
@@ -1707,10 +1794,10 @@
     </row>
     <row r="45" spans="1:7" ht="14" thickBot="1">
       <c r="A45" s="3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="C45" s="5">
         <v>40073</v>
@@ -1727,10 +1814,10 @@
     </row>
     <row r="46" spans="1:7" ht="14" thickBot="1">
       <c r="A46" s="3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C46" s="5">
         <v>40073</v>
@@ -1747,10 +1834,10 @@
     </row>
     <row r="47" spans="1:7" ht="14" thickBot="1">
       <c r="A47" s="3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="C47" s="5">
         <v>40075</v>
@@ -1767,10 +1854,10 @@
     </row>
     <row r="48" spans="1:7" ht="14" thickBot="1">
       <c r="A48" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="C48" s="5">
         <v>40077</v>
@@ -1787,10 +1874,10 @@
     </row>
     <row r="49" spans="1:7" ht="14" thickBot="1">
       <c r="A49" s="3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="C49" s="5">
         <v>40077</v>
@@ -1807,10 +1894,10 @@
     </row>
     <row r="50" spans="1:7" ht="14" thickBot="1">
       <c r="A50" s="3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="C50" s="5">
         <v>40078</v>
@@ -1827,10 +1914,10 @@
     </row>
     <row r="51" spans="1:7" ht="14" thickBot="1">
       <c r="A51" s="3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C51" s="5">
         <v>40079</v>
@@ -1847,10 +1934,10 @@
     </row>
     <row r="52" spans="1:7" ht="14" thickBot="1">
       <c r="A52" s="3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="C52" s="5">
         <v>40079</v>
@@ -1866,6 +1953,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C2:C52">
     <cfRule type="expression" dxfId="1" priority="0" stopIfTrue="1">

</xml_diff>

<commit_message>
update tasks and status
</commit_message>
<xml_diff>
--- a/Documentation/Project1TasksSpreadsheet.xlsx
+++ b/Documentation/Project1TasksSpreadsheet.xlsx
@@ -794,7 +794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="125" workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -1923,7 +1923,7 @@
         <v>40078</v>
       </c>
       <c r="D50" s="13">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E50" s="9"/>
       <c r="F50" s="6"/>
@@ -1973,6 +1973,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C2:C52">
     <cfRule type="expression" dxfId="1" priority="0" stopIfTrue="1">

</xml_diff>

<commit_message>
Updating new project code for motor control GUI, Jerrell's android code, and Tasks
</commit_message>
<xml_diff>
--- a/Documentation/Project1TasksSpreadsheet.xlsx
+++ b/Documentation/Project1TasksSpreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="33960" windowHeight="22440" tabRatio="500"/>
+    <workbookView xWindow="-60" yWindow="20" windowWidth="33960" windowHeight="22440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,107 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
+  <si>
+    <t>Code Hello World Tablet</t>
+  </si>
+  <si>
+    <t>Test Hello World Tablet</t>
+  </si>
+  <si>
+    <t>Code Hello World Phone</t>
+  </si>
+  <si>
+    <t>Test Hello World Phone</t>
+  </si>
+  <si>
+    <t>Ensure all devices are secured in storage</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <t>Find motor spec sheets</t>
+  </si>
+  <si>
+    <t>Build Robot Frame</t>
+  </si>
+  <si>
+    <t>Code individual motor motion</t>
+  </si>
+  <si>
+    <t>Test individual motor motion</t>
+  </si>
+  <si>
+    <t>Create methods for moving robot forward/backward</t>
+  </si>
+  <si>
+    <t>Create methods for moving robot left/right</t>
+  </si>
+  <si>
+    <t>Test forward/backward motion</t>
+  </si>
+  <si>
+    <t>Test left/right motion</t>
+  </si>
+  <si>
+    <t>Determine sensors necessary to avoid obstacles</t>
+  </si>
+  <si>
+    <t>Find necessary references on sensors</t>
+  </si>
+  <si>
+    <t>Code object avoidance</t>
+  </si>
+  <si>
+    <t>Wi-Fi seems best at the moment using ssh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>App development in progress. Learning on the fly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test obstacle avoidance</t>
+  </si>
+  <si>
+    <t>Choose communication medium between Phone/Tablet</t>
+  </si>
+  <si>
+    <t>Learn to use this medium for android</t>
+  </si>
+  <si>
+    <t>Merge Project code to final projects for submittal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Report</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jacob</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jerrell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Presentation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sei Jung</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interrupt based Obstacle Avoidance and dynamic IP setting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Write communication code</t>
   </si>
@@ -141,49 +241,13 @@
     <t>Learn to set up/compile code for Vex</t>
   </si>
   <si>
-    <t>Object Avoidance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Android end of Vex-android communication</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vex end of Vex-android communication</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Controller</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Report</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Grade Movement</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Jerrell</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learn to operate/code in Debian Linux</t>
   </si>
   <si>
     <t>Alex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sei Jung/Jacob</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jerrell</t>
-  </si>
-  <si>
-    <t>Learn to operate/code in Debian Linux</t>
-  </si>
-  <si>
-    <t>Alex</t>
   </si>
   <si>
     <t>Learn to program ARM9 processor</t>
@@ -208,81 +272,17 @@
   </si>
   <si>
     <t>Make sure tablet interfaces correctly with computer</t>
-  </si>
-  <si>
-    <t>Code Hello World Tablet</t>
-  </si>
-  <si>
-    <t>Test Hello World Tablet</t>
-  </si>
-  <si>
-    <t>Code Hello World Phone</t>
-  </si>
-  <si>
-    <t>Test Hello World Phone</t>
-  </si>
-  <si>
-    <t>Ensure all devices are secured in storage</t>
-  </si>
-  <si>
-    <t>ongoing</t>
-  </si>
-  <si>
-    <t>Find motor spec sheets</t>
-  </si>
-  <si>
-    <t>Build Robot Frame</t>
-  </si>
-  <si>
-    <t>Code individual motor motion</t>
-  </si>
-  <si>
-    <t>Test individual motor motion</t>
-  </si>
-  <si>
-    <t>Create methods for moving robot forward/backward</t>
-  </si>
-  <si>
-    <t>Create methods for moving robot left/right</t>
-  </si>
-  <si>
-    <t>Test forward/backward motion</t>
-  </si>
-  <si>
-    <t>Test left/right motion</t>
-  </si>
-  <si>
-    <t>Determine sensors necessary to avoid obstacles</t>
-  </si>
-  <si>
-    <t>Find necessary references on sensors</t>
-  </si>
-  <si>
-    <t>Code object avoidance</t>
-  </si>
-  <si>
-    <t>Wi-Fi seems best at the moment using ssh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>App development in progress. Learning on the fly</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test obstacle avoidance</t>
-  </si>
-  <si>
-    <t>Choose communication medium between Phone/Tablet</t>
-  </si>
-  <si>
-    <t>Learn to use this medium for android</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="5">
@@ -792,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -808,37 +808,37 @@
   <sheetData>
     <row r="1" spans="1:8" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H1" s="7">
         <f ca="1">TODAY()</f>
-        <v>40075</v>
+        <v>40079</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14" thickBot="1">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C2" s="5">
         <v>40059</v>
@@ -857,10 +857,10 @@
     </row>
     <row r="3" spans="1:8" ht="14" thickBot="1">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="C3" s="5">
         <v>40059</v>
@@ -873,16 +873,16 @@
       </c>
       <c r="F3" s="6"/>
       <c r="G3">
-        <f t="shared" ref="G3:G52" ca="1" si="0">IF(AND(C3&lt;$H$1,D3&lt;1),1,0)</f>
+        <f t="shared" ref="G3:G58" ca="1" si="0">IF(AND(C3&lt;$H$1,D3&lt;1),1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="C4" s="5">
         <v>40059</v>
@@ -901,10 +901,10 @@
     </row>
     <row r="5" spans="1:8" ht="14" thickBot="1">
       <c r="A5" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="C5" s="5">
         <v>40059</v>
@@ -923,10 +923,10 @@
     </row>
     <row r="6" spans="1:8" ht="14" thickBot="1">
       <c r="A6" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="C6" s="5">
         <v>40059</v>
@@ -945,10 +945,10 @@
     </row>
     <row r="7" spans="1:8" ht="14" thickBot="1">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="C7" s="5">
         <v>40060</v>
@@ -967,10 +967,10 @@
     </row>
     <row r="8" spans="1:8" ht="14" thickBot="1">
       <c r="A8" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="C8" s="5">
         <v>40060</v>
@@ -989,10 +989,10 @@
     </row>
     <row r="9" spans="1:8" ht="14" thickBot="1">
       <c r="A9" s="3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="C9" s="5">
         <v>40061</v>
@@ -1011,10 +1011,10 @@
     </row>
     <row r="10" spans="1:8" ht="14" thickBot="1">
       <c r="A10" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="C10" s="5">
         <v>40061</v>
@@ -1033,10 +1033,10 @@
     </row>
     <row r="11" spans="1:8" ht="14" thickBot="1">
       <c r="A11" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C11" s="5">
         <v>40061</v>
@@ -1055,10 +1055,10 @@
     </row>
     <row r="12" spans="1:8" ht="14" thickBot="1">
       <c r="A12" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="C12" s="5">
         <v>40061</v>
@@ -1077,10 +1077,10 @@
     </row>
     <row r="13" spans="1:8" ht="14" thickBot="1">
       <c r="A13" s="3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="C13" s="5">
         <v>40061</v>
@@ -1099,10 +1099,10 @@
     </row>
     <row r="14" spans="1:8" ht="14" thickBot="1">
       <c r="A14" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>59</v>
+        <v>2</v>
       </c>
       <c r="C14" s="5">
         <v>40061</v>
@@ -1121,10 +1121,10 @@
     </row>
     <row r="15" spans="1:8" ht="14" thickBot="1">
       <c r="A15" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C15" s="5">
         <v>40061</v>
@@ -1143,10 +1143,10 @@
     </row>
     <row r="16" spans="1:8" ht="14" thickBot="1">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="C16" s="5">
         <v>40063</v>
@@ -1163,15 +1163,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14" thickBot="1">
+    <row r="17" spans="1:7" ht="14" thickBot="1">
       <c r="A17" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="D17" s="13">
         <v>0</v>
@@ -1183,12 +1183,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14" thickBot="1">
+    <row r="18" spans="1:7" ht="14" thickBot="1">
       <c r="A18" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C18" s="5">
         <v>40063</v>
@@ -1205,12 +1205,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14" thickBot="1">
+    <row r="19" spans="1:7" ht="14" thickBot="1">
       <c r="A19" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="C19" s="5">
         <v>40061</v>
@@ -1227,12 +1227,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14" thickBot="1">
+    <row r="20" spans="1:7" ht="14" thickBot="1">
       <c r="A20" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="C20" s="5">
         <v>40063</v>
@@ -1249,12 +1249,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14" thickBot="1">
+    <row r="21" spans="1:7" ht="14" thickBot="1">
       <c r="A21" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="C21" s="5">
         <v>40063</v>
@@ -1271,12 +1271,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14" thickBot="1">
+    <row r="22" spans="1:7" ht="14" thickBot="1">
       <c r="A22" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C22" s="5">
         <v>40063</v>
@@ -1293,12 +1293,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14" thickBot="1">
+    <row r="23" spans="1:7" ht="14" thickBot="1">
       <c r="A23" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="C23" s="5">
         <v>40063</v>
@@ -1315,12 +1315,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14" thickBot="1">
+    <row r="24" spans="1:7" ht="14" thickBot="1">
       <c r="A24" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="C24" s="5">
         <v>40063</v>
@@ -1332,19 +1332,19 @@
         <v>40062</v>
       </c>
       <c r="F24" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="14" thickBot="1">
+      <c r="A25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="G24">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="14" thickBot="1">
-      <c r="A25" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="C25" s="5">
         <v>40063</v>
@@ -1361,12 +1361,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14" thickBot="1">
+    <row r="26" spans="1:7" ht="14" thickBot="1">
       <c r="A26" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="C26" s="5">
         <v>40066</v>
@@ -1378,19 +1378,19 @@
         <v>40062</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="14" thickBot="1">
+    <row r="27" spans="1:7" ht="14" thickBot="1">
       <c r="A27" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="C27" s="5">
         <v>40066</v>
@@ -1404,19 +1404,13 @@
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="H27" t="s">
-        <v>44</v>
-      </c>
-      <c r="I27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="14" thickBot="1">
+    </row>
+    <row r="28" spans="1:7" ht="14" thickBot="1">
       <c r="A28" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="C28" s="5">
         <v>40069</v>
@@ -1430,19 +1424,13 @@
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-      <c r="H28" t="s">
-        <v>45</v>
-      </c>
-      <c r="I28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="14" thickBot="1">
+    </row>
+    <row r="29" spans="1:7" ht="14" thickBot="1">
       <c r="A29" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="C29" s="5">
         <v>40070</v>
@@ -1456,19 +1444,13 @@
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-      <c r="H29" t="s">
-        <v>44</v>
-      </c>
-      <c r="I29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="14" thickBot="1">
+    </row>
+    <row r="30" spans="1:7" ht="14" thickBot="1">
       <c r="A30" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="C30" s="5">
         <v>40061</v>
@@ -1480,22 +1462,19 @@
         <v>40062</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="I30" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="14" thickBot="1">
+    </row>
+    <row r="31" spans="1:7" ht="14" thickBot="1">
       <c r="A31" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="C31" s="5">
         <v>40066</v>
@@ -1511,19 +1490,13 @@
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="H31" t="s">
-        <v>44</v>
-      </c>
-      <c r="I31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="14" thickBot="1">
+    </row>
+    <row r="32" spans="1:7" ht="14" thickBot="1">
       <c r="A32" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C32" s="5">
         <v>40069</v>
@@ -1535,25 +1508,19 @@
         <v>40066</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
-      </c>
-      <c r="H32" t="s">
-        <v>43</v>
-      </c>
-      <c r="I32" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="14" thickBot="1">
       <c r="A33" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C33" s="5">
         <v>40070</v>
@@ -1572,10 +1539,10 @@
     </row>
     <row r="34" spans="1:7" ht="14" thickBot="1">
       <c r="A34" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C34" s="5">
         <v>40061</v>
@@ -1587,7 +1554,7 @@
         <v>40067</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="0"/>
@@ -1596,10 +1563,10 @@
     </row>
     <row r="35" spans="1:7" ht="14" thickBot="1">
       <c r="A35" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="C35" s="5">
         <v>40066</v>
@@ -1609,7 +1576,7 @@
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="6" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="0"/>
@@ -1618,96 +1585,96 @@
     </row>
     <row r="36" spans="1:7" ht="14" thickBot="1">
       <c r="A36" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C36" s="5">
         <v>40069</v>
       </c>
       <c r="D36" s="13">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="6"/>
       <c r="G36">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="14" thickBot="1">
       <c r="A37" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>4</v>
       </c>
       <c r="C37" s="5">
         <v>40070</v>
       </c>
       <c r="D37" s="13">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="6"/>
       <c r="G37">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="14" thickBot="1">
       <c r="A38" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C38" s="5">
         <v>40073</v>
       </c>
       <c r="D38" s="13">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="6"/>
       <c r="G38">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="14" thickBot="1">
       <c r="A39" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C39" s="5">
         <v>40074</v>
       </c>
       <c r="D39" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="6"/>
       <c r="G39">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="14" thickBot="1">
       <c r="A40" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C40" s="5">
         <v>40076</v>
       </c>
       <c r="D40" s="13">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E40" s="9"/>
       <c r="F40" s="6"/>
@@ -1718,30 +1685,30 @@
     </row>
     <row r="41" spans="1:7" ht="14" thickBot="1">
       <c r="A41" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C41" s="5">
         <v>40076</v>
       </c>
       <c r="D41" s="13">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="6"/>
       <c r="G41">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="14" thickBot="1">
       <c r="A42" s="3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C42" s="5">
         <v>40063</v>
@@ -1750,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="F42" s="6"/>
       <c r="G42">
@@ -1760,10 +1727,10 @@
     </row>
     <row r="43" spans="1:7" ht="14" thickBot="1">
       <c r="A43" s="3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="C43" s="5">
         <v>40069</v>
@@ -1772,7 +1739,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="F43" s="6"/>
       <c r="G43">
@@ -1782,10 +1749,10 @@
     </row>
     <row r="44" spans="1:7" ht="14" thickBot="1">
       <c r="A44" s="3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C44" s="5">
         <v>40069</v>
@@ -1794,7 +1761,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="F44" s="6"/>
       <c r="G44">
@@ -1804,10 +1771,10 @@
     </row>
     <row r="45" spans="1:7" ht="14" thickBot="1">
       <c r="A45" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="C45" s="5">
         <v>40073</v>
@@ -1816,7 +1783,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="F45" s="6"/>
       <c r="G45">
@@ -1826,10 +1793,10 @@
     </row>
     <row r="46" spans="1:7" ht="14" thickBot="1">
       <c r="A46" s="3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C46" s="5">
         <v>40073</v>
@@ -1838,7 +1805,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46">
@@ -1848,10 +1815,10 @@
     </row>
     <row r="47" spans="1:7" ht="14" thickBot="1">
       <c r="A47" s="3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C47" s="5">
         <v>40075</v>
@@ -1860,7 +1827,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="F47" s="6"/>
       <c r="G47">
@@ -1870,10 +1837,10 @@
     </row>
     <row r="48" spans="1:7" ht="14" thickBot="1">
       <c r="A48" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C48" s="5">
         <v>40077</v>
@@ -1882,7 +1849,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48">
@@ -1892,10 +1859,10 @@
     </row>
     <row r="49" spans="1:7" ht="14" thickBot="1">
       <c r="A49" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C49" s="5">
         <v>40077</v>
@@ -1904,7 +1871,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49">
@@ -1914,10 +1881,10 @@
     </row>
     <row r="50" spans="1:7" ht="14" thickBot="1">
       <c r="A50" s="3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C50" s="5">
         <v>40078</v>
@@ -1934,16 +1901,16 @@
     </row>
     <row r="51" spans="1:7" ht="14" thickBot="1">
       <c r="A51" s="3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C51" s="5">
         <v>40079</v>
       </c>
       <c r="D51" s="13">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E51" s="9"/>
       <c r="F51" s="6"/>
@@ -1954,28 +1921,124 @@
     </row>
     <row r="52" spans="1:7" ht="14" thickBot="1">
       <c r="A52" s="3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C52" s="5">
         <v>40079</v>
       </c>
-      <c r="D52" s="14">
-        <v>0.9</v>
-      </c>
-      <c r="E52" s="10"/>
-      <c r="F52" s="5"/>
+      <c r="D52" s="13">
+        <v>1</v>
+      </c>
+      <c r="E52" s="9"/>
+      <c r="F52" s="6"/>
       <c r="G52">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="53" spans="1:7" ht="14" thickBot="1">
+      <c r="A53" s="3"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="1:7" ht="14" thickBot="1">
+      <c r="A54" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" s="5">
+        <v>40080</v>
+      </c>
+      <c r="D54" s="13">
+        <v>0</v>
+      </c>
+      <c r="E54" s="9"/>
+      <c r="F54" s="6"/>
+      <c r="G54">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="14" thickBot="1">
+      <c r="A55" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" s="5">
+        <v>40080</v>
+      </c>
+      <c r="D55" s="13">
+        <v>0</v>
+      </c>
+      <c r="E55" s="9"/>
+      <c r="F55" s="6"/>
+      <c r="G55">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="14" thickBot="1">
+      <c r="A56" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" s="5">
+        <v>40080</v>
+      </c>
+      <c r="D56" s="13">
+        <v>0</v>
+      </c>
+      <c r="E56" s="9"/>
+      <c r="F56" s="6"/>
+      <c r="G56">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="14" thickBot="1">
+      <c r="A57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="5">
+        <v>40080</v>
+      </c>
+      <c r="D57" s="13">
+        <v>0</v>
+      </c>
+      <c r="E57" s="9"/>
+      <c r="F57" s="6"/>
+      <c r="G57">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="14" thickBot="1">
+      <c r="A58" s="3"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="5"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C2:C52">
+  <conditionalFormatting sqref="C2:C58">
     <cfRule type="expression" dxfId="1" priority="0" stopIfTrue="1">
       <formula>G2=1</formula>
     </cfRule>
@@ -1984,6 +2047,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>